<commit_message>
got rid of village, quarry, forest
to fg1 etc
</commit_message>
<xml_diff>
--- a/Data/LandCover/Watershed_Stats.xlsx
+++ b/Data/LandCover/Watershed_Stats.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fagaalu" sheetId="1" r:id="rId1"/>
-    <sheet name="Nuuuli" sheetId="2" r:id="rId2"/>
+    <sheet name="Fagaalu_Revised" sheetId="3" r:id="rId2"/>
+    <sheet name="Nuuuli" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Watershed</t>
   </si>
@@ -148,6 +149,18 @@
   </si>
   <si>
     <t>Fagaalu Stream</t>
+  </si>
+  <si>
+    <t>QUARRY(LOWER)</t>
+  </si>
+  <si>
+    <t>VILLAGE(LOWER)</t>
+  </si>
+  <si>
+    <t>% of area</t>
+  </si>
+  <si>
+    <t>Cumulative %</t>
   </si>
 </sst>
 </file>
@@ -303,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -358,6 +371,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,11 +655,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +667,7 @@
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="8" width="11.42578125" customWidth="1"/>
@@ -1320,6 +1334,498 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="48" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" s="48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="31">
+        <v>0.89724999999999999</v>
+      </c>
+      <c r="C2" s="33">
+        <f>B2/$B$5</f>
+        <v>0.48221306911622125</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0.48</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="34">
+        <v>476</v>
+      </c>
+      <c r="J2" s="34">
+        <v>739484</v>
+      </c>
+      <c r="K2" s="34">
+        <v>153685</v>
+      </c>
+      <c r="L2" s="34">
+        <v>3574</v>
+      </c>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34">
+        <f t="shared" ref="N2:N6" si="0">SUM(F2:M2)</f>
+        <v>897219</v>
+      </c>
+      <c r="O2" s="35">
+        <f>F2/$N2</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="35">
+        <f>G2/$N2</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="35">
+        <f>H2/$N2</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="35">
+        <f>I2/$N2</f>
+        <v>5.3052822109206333E-4</v>
+      </c>
+      <c r="S2" s="35">
+        <f>J2/$N2</f>
+        <v>0.82419565345807433</v>
+      </c>
+      <c r="T2" s="35">
+        <f>K2/$N2</f>
+        <v>0.17129039844229782</v>
+      </c>
+      <c r="U2" s="35">
+        <f>L2/$N2</f>
+        <v>3.9834198785357868E-3</v>
+      </c>
+      <c r="V2" s="36">
+        <f>M2/$N2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1.171996</v>
+      </c>
+      <c r="C3" s="28">
+        <f>B3/$B$5</f>
+        <v>0.62987103722701021</v>
+      </c>
+      <c r="D3" s="26">
+        <v>0.27474600000000005</v>
+      </c>
+      <c r="E3" s="27">
+        <f>0.27/1.86</f>
+        <v>0.14516129032258066</v>
+      </c>
+      <c r="F3" s="25">
+        <f>2008-F2</f>
+        <v>2008</v>
+      </c>
+      <c r="G3" s="25">
+        <f>348-G2</f>
+        <v>348</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25">
+        <f>1816-I2</f>
+        <v>1340</v>
+      </c>
+      <c r="J3" s="25">
+        <f>992494-J2</f>
+        <v>253010</v>
+      </c>
+      <c r="K3" s="25">
+        <f>156112-K2</f>
+        <v>2427</v>
+      </c>
+      <c r="L3" s="25">
+        <f>19204-L2</f>
+        <v>15630</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25">
+        <f t="shared" si="0"/>
+        <v>274763</v>
+      </c>
+      <c r="O3" s="29">
+        <f>F3/$N3</f>
+        <v>7.3081164494491618E-3</v>
+      </c>
+      <c r="P3" s="29">
+        <f>G3/$N3</f>
+        <v>1.2665460778925838E-3</v>
+      </c>
+      <c r="Q3" s="29">
+        <f>H3/$N3</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="29">
+        <f>I3/$N3</f>
+        <v>4.8769302999312134E-3</v>
+      </c>
+      <c r="S3" s="29">
+        <f>J3/$N3</f>
+        <v>0.92082995163104198</v>
+      </c>
+      <c r="T3" s="29">
+        <f>K3/$N3</f>
+        <v>8.8330670432336233E-3</v>
+      </c>
+      <c r="U3" s="29">
+        <f>L3/$N3</f>
+        <v>5.6885388498451393E-2</v>
+      </c>
+      <c r="V3" s="30">
+        <f>M3/$N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="37">
+        <v>1.776413</v>
+      </c>
+      <c r="C4" s="39">
+        <f>B4/$B$5</f>
+        <v>0.95470556115681693</v>
+      </c>
+      <c r="D4" s="37">
+        <f>B4-B3</f>
+        <v>0.60441699999999998</v>
+      </c>
+      <c r="E4" s="38">
+        <f>D4/1.86</f>
+        <v>0.324955376344086</v>
+      </c>
+      <c r="F4" s="40">
+        <f>56406-F3</f>
+        <v>54398</v>
+      </c>
+      <c r="G4" s="40">
+        <f>16249-G3</f>
+        <v>15901</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="40">
+        <f>2874-I3</f>
+        <v>1534</v>
+      </c>
+      <c r="J4" s="40">
+        <f>1521947-J3</f>
+        <v>1268937</v>
+      </c>
+      <c r="K4" s="40">
+        <f>159545-K3</f>
+        <v>157118</v>
+      </c>
+      <c r="L4" s="40">
+        <f>19379-L3</f>
+        <v>3749</v>
+      </c>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40">
+        <f t="shared" si="0"/>
+        <v>1501637</v>
+      </c>
+      <c r="O4" s="41">
+        <f>F4/$N4</f>
+        <v>3.6225798911454631E-2</v>
+      </c>
+      <c r="P4" s="41">
+        <f>G4/$N4</f>
+        <v>1.0589110417497704E-2</v>
+      </c>
+      <c r="Q4" s="41">
+        <f>H4/$N4</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="41">
+        <f>I4/$N4</f>
+        <v>1.0215518131212803E-3</v>
+      </c>
+      <c r="S4" s="41">
+        <f>J4/$N4</f>
+        <v>0.84503578428075499</v>
+      </c>
+      <c r="T4" s="41">
+        <f>K4/$N4</f>
+        <v>0.10463114587613384</v>
+      </c>
+      <c r="U4" s="41">
+        <f>L4/$N4</f>
+        <v>2.4966087010376008E-3</v>
+      </c>
+      <c r="V4" s="42">
+        <f>M4/$N4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="43">
+        <v>1.860692</v>
+      </c>
+      <c r="C5" s="45">
+        <f>B5/$B$5</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="43">
+        <v>8.4278999999999993E-2</v>
+      </c>
+      <c r="E5" s="44">
+        <v>4.5294438843183071E-2</v>
+      </c>
+      <c r="F5" s="13">
+        <v>85528</v>
+      </c>
+      <c r="G5" s="13">
+        <v>21192</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13">
+        <v>2874</v>
+      </c>
+      <c r="J5" s="13">
+        <v>1571530</v>
+      </c>
+      <c r="K5" s="13">
+        <v>160179</v>
+      </c>
+      <c r="L5" s="13">
+        <v>19379</v>
+      </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13">
+        <f t="shared" si="0"/>
+        <v>1860682</v>
+      </c>
+      <c r="O5" s="46">
+        <f>F5/$N5</f>
+        <v>4.5965941520367266E-2</v>
+      </c>
+      <c r="P5" s="46">
+        <f>G5/$N5</f>
+        <v>1.1389372283926001E-2</v>
+      </c>
+      <c r="Q5" s="46">
+        <f>H5/$N5</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="46">
+        <f>I5/$N5</f>
+        <v>1.5445949388450042E-3</v>
+      </c>
+      <c r="S5" s="46">
+        <f>J5/$N5</f>
+        <v>0.84459891588138114</v>
+      </c>
+      <c r="T5" s="46">
+        <f>K5/$N5</f>
+        <v>8.608617700391577E-2</v>
+      </c>
+      <c r="U5" s="46">
+        <f>L5/$N5</f>
+        <v>1.0414998371564834E-2</v>
+      </c>
+      <c r="V5" s="47">
+        <f>M5/$N5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.4778150000000001</v>
+      </c>
+      <c r="D6" s="3">
+        <f>SUM(D2:D5)</f>
+        <v>1.863442</v>
+      </c>
+      <c r="E6" s="50">
+        <f>SUM(E2:E5)</f>
+        <v>0.99541110550984968</v>
+      </c>
+      <c r="F6">
+        <v>177490</v>
+      </c>
+      <c r="G6">
+        <v>61384</v>
+      </c>
+      <c r="H6">
+        <v>11447</v>
+      </c>
+      <c r="I6">
+        <v>7294</v>
+      </c>
+      <c r="J6">
+        <v>2024813</v>
+      </c>
+      <c r="K6">
+        <v>166192</v>
+      </c>
+      <c r="L6">
+        <v>26936</v>
+      </c>
+      <c r="M6">
+        <v>2269</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>2477825</v>
+      </c>
+      <c r="O6" s="1">
+        <f>F6/$N6</f>
+        <v>7.163137025415435E-2</v>
+      </c>
+      <c r="P6" s="1">
+        <f>G6/$N6</f>
+        <v>2.4773339521556203E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>H6/$N6</f>
+        <v>4.619777425766549E-3</v>
+      </c>
+      <c r="R6" s="1">
+        <f>I6/$N6</f>
+        <v>2.9437107140334769E-3</v>
+      </c>
+      <c r="S6" s="1">
+        <f>J6/$N6</f>
+        <v>0.81717352920403985</v>
+      </c>
+      <c r="T6" s="1">
+        <f>K6/$N6</f>
+        <v>6.7071726211495972E-2</v>
+      </c>
+      <c r="U6" s="1">
+        <f>L6/$N6</f>
+        <v>1.0870824210749346E-2</v>
+      </c>
+      <c r="V6" s="1">
+        <f>M6/$N6</f>
+        <v>9.1572245820427194E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>

</xml_diff>

<commit_message>
halfway through first revision from Trent
changed Q vs C, box plots etc
</commit_message>
<xml_diff>
--- a/Data/LandCover/Watershed_Stats.xlsx
+++ b/Data/LandCover/Watershed_Stats.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
   <si>
     <t>Watershed</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Cumulative %</t>
+  </si>
+  <si>
+    <t>% Undisturbed</t>
+  </si>
+  <si>
+    <t>% Disturbed</t>
   </si>
 </sst>
 </file>
@@ -316,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -372,6 +378,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1335,13 +1347,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,17 +1370,19 @@
     <col min="11" max="11" width="7.5703125" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="8.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" customWidth="1"/>
-    <col min="20" max="20" width="7.7109375" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" customWidth="1"/>
     <col min="22" max="22" width="8.140625" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="48" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="48" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>35</v>
       </c>
@@ -1412,31 +1426,37 @@
         <v>19</v>
       </c>
       <c r="O1" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="Q1" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="R1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="S1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="T1" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="U1" s="49" t="s">
         <v>34</v>
-      </c>
-      <c r="U1" s="48" t="s">
-        <v>33</v>
       </c>
       <c r="V1" s="48" t="s">
         <v>9</v>
       </c>
+      <c r="W1" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>36</v>
       </c>
@@ -1474,39 +1494,48 @@
         <v>897219</v>
       </c>
       <c r="O2" s="35">
-        <f>F2/$N2</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="35">
-        <f>G2/$N2</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" s="35">
-        <f>H2/$N2</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="35">
-        <f>I2/$N2</f>
-        <v>5.3052822109206333E-4</v>
-      </c>
-      <c r="S2" s="35">
-        <f>J2/$N2</f>
-        <v>0.82419565345807433</v>
-      </c>
-      <c r="T2" s="35">
-        <f>K2/$N2</f>
-        <v>0.17129039844229782</v>
-      </c>
-      <c r="U2" s="35">
         <f>L2/$N2</f>
         <v>3.9834198785357868E-3</v>
       </c>
+      <c r="P2" s="35">
+        <f t="shared" ref="P2:U6" si="1">F2/$N2</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R2" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S2" s="35">
+        <f t="shared" si="1"/>
+        <v>5.3052822109206333E-4</v>
+      </c>
+      <c r="T2" s="35">
+        <f t="shared" si="1"/>
+        <v>0.82419565345807433</v>
+      </c>
+      <c r="U2" s="35">
+        <f t="shared" si="1"/>
+        <v>0.17129039844229782</v>
+      </c>
       <c r="V2" s="36">
         <f>M2/$N2</f>
         <v>0</v>
       </c>
+      <c r="W2" s="51">
+        <f>SUM(L2,F2:G2)/N2</f>
+        <v>3.9834198785357868E-3</v>
+      </c>
+      <c r="X2" s="1">
+        <f>SUM(I2:K2)/N2</f>
+        <v>0.99601658012146421</v>
+      </c>
+      <c r="Y2" s="54"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>41</v>
       </c>
@@ -1555,39 +1584,48 @@
         <v>274763</v>
       </c>
       <c r="O3" s="29">
-        <f>F3/$N3</f>
-        <v>7.3081164494491618E-3</v>
-      </c>
-      <c r="P3" s="29">
-        <f>G3/$N3</f>
-        <v>1.2665460778925838E-3</v>
-      </c>
-      <c r="Q3" s="29">
-        <f>H3/$N3</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="29">
-        <f>I3/$N3</f>
-        <v>4.8769302999312134E-3</v>
-      </c>
-      <c r="S3" s="29">
-        <f>J3/$N3</f>
-        <v>0.92082995163104198</v>
-      </c>
-      <c r="T3" s="29">
-        <f>K3/$N3</f>
-        <v>8.8330670432336233E-3</v>
-      </c>
-      <c r="U3" s="29">
         <f>L3/$N3</f>
         <v>5.6885388498451393E-2</v>
       </c>
+      <c r="P3" s="29">
+        <f t="shared" si="1"/>
+        <v>7.3081164494491618E-3</v>
+      </c>
+      <c r="Q3" s="29">
+        <f t="shared" si="1"/>
+        <v>1.2665460778925838E-3</v>
+      </c>
+      <c r="R3" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S3" s="29">
+        <f t="shared" si="1"/>
+        <v>4.8769302999312134E-3</v>
+      </c>
+      <c r="T3" s="29">
+        <f t="shared" si="1"/>
+        <v>0.92082995163104198</v>
+      </c>
+      <c r="U3" s="29">
+        <f t="shared" si="1"/>
+        <v>8.8330670432336233E-3</v>
+      </c>
       <c r="V3" s="30">
         <f>M3/$N3</f>
         <v>0</v>
       </c>
+      <c r="W3" s="51">
+        <f t="shared" ref="W3:W5" si="2">SUM(L3,F3:G3)/N3</f>
+        <v>6.5460051025793137E-2</v>
+      </c>
+      <c r="X3" s="1">
+        <f t="shared" ref="X3:X6" si="3">SUM(I3:K3)/N3</f>
+        <v>0.93453994897420689</v>
+      </c>
+      <c r="Y3" s="54"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>42</v>
       </c>
@@ -1637,39 +1675,48 @@
         <v>1501637</v>
       </c>
       <c r="O4" s="41">
-        <f>F4/$N4</f>
-        <v>3.6225798911454631E-2</v>
-      </c>
-      <c r="P4" s="41">
-        <f>G4/$N4</f>
-        <v>1.0589110417497704E-2</v>
-      </c>
-      <c r="Q4" s="41">
-        <f>H4/$N4</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="41">
-        <f>I4/$N4</f>
-        <v>1.0215518131212803E-3</v>
-      </c>
-      <c r="S4" s="41">
-        <f>J4/$N4</f>
-        <v>0.84503578428075499</v>
-      </c>
-      <c r="T4" s="41">
-        <f>K4/$N4</f>
-        <v>0.10463114587613384</v>
-      </c>
-      <c r="U4" s="41">
         <f>L4/$N4</f>
         <v>2.4966087010376008E-3</v>
       </c>
+      <c r="P4" s="41">
+        <f t="shared" si="1"/>
+        <v>3.6225798911454631E-2</v>
+      </c>
+      <c r="Q4" s="41">
+        <f t="shared" si="1"/>
+        <v>1.0589110417497704E-2</v>
+      </c>
+      <c r="R4" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="41">
+        <f t="shared" si="1"/>
+        <v>1.0215518131212803E-3</v>
+      </c>
+      <c r="T4" s="41">
+        <f t="shared" si="1"/>
+        <v>0.84503578428075499</v>
+      </c>
+      <c r="U4" s="41">
+        <f t="shared" si="1"/>
+        <v>0.10463114587613384</v>
+      </c>
       <c r="V4" s="42">
         <f>M4/$N4</f>
         <v>0</v>
       </c>
+      <c r="W4" s="51">
+        <f t="shared" si="2"/>
+        <v>4.931151802998994E-2</v>
+      </c>
+      <c r="X4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.9506884819700101</v>
+      </c>
+      <c r="Y4" s="54"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>40</v>
       </c>
@@ -1711,39 +1758,48 @@
         <v>1860682</v>
       </c>
       <c r="O5" s="46">
-        <f>F5/$N5</f>
-        <v>4.5965941520367266E-2</v>
-      </c>
-      <c r="P5" s="46">
-        <f>G5/$N5</f>
-        <v>1.1389372283926001E-2</v>
-      </c>
-      <c r="Q5" s="46">
-        <f>H5/$N5</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="46">
-        <f>I5/$N5</f>
-        <v>1.5445949388450042E-3</v>
-      </c>
-      <c r="S5" s="46">
-        <f>J5/$N5</f>
-        <v>0.84459891588138114</v>
-      </c>
-      <c r="T5" s="46">
-        <f>K5/$N5</f>
-        <v>8.608617700391577E-2</v>
-      </c>
-      <c r="U5" s="46">
         <f>L5/$N5</f>
         <v>1.0414998371564834E-2</v>
       </c>
+      <c r="P5" s="46">
+        <f t="shared" si="1"/>
+        <v>4.5965941520367266E-2</v>
+      </c>
+      <c r="Q5" s="46">
+        <f t="shared" si="1"/>
+        <v>1.1389372283926001E-2</v>
+      </c>
+      <c r="R5" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="46">
+        <f t="shared" si="1"/>
+        <v>1.5445949388450042E-3</v>
+      </c>
+      <c r="T5" s="46">
+        <f t="shared" si="1"/>
+        <v>0.84459891588138114</v>
+      </c>
+      <c r="U5" s="46">
+        <f t="shared" si="1"/>
+        <v>8.608617700391577E-2</v>
+      </c>
       <c r="V5" s="47">
         <f>M5/$N5</f>
         <v>0</v>
       </c>
+      <c r="W5" s="51">
+        <f t="shared" si="2"/>
+        <v>6.7770312175858105E-2</v>
+      </c>
+      <c r="X5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.93222968782414195</v>
+      </c>
+      <c r="Y5" s="54"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1787,37 +1843,46 @@
         <v>2477825</v>
       </c>
       <c r="O6" s="1">
-        <f>F6/$N6</f>
-        <v>7.163137025415435E-2</v>
-      </c>
-      <c r="P6" s="1">
-        <f>G6/$N6</f>
-        <v>2.4773339521556203E-2</v>
-      </c>
-      <c r="Q6" s="1">
-        <f>H6/$N6</f>
-        <v>4.619777425766549E-3</v>
-      </c>
-      <c r="R6" s="1">
-        <f>I6/$N6</f>
-        <v>2.9437107140334769E-3</v>
-      </c>
-      <c r="S6" s="1">
-        <f>J6/$N6</f>
-        <v>0.81717352920403985</v>
-      </c>
-      <c r="T6" s="1">
-        <f>K6/$N6</f>
-        <v>6.7071726211495972E-2</v>
-      </c>
-      <c r="U6" s="1">
         <f>L6/$N6</f>
         <v>1.0870824210749346E-2</v>
+      </c>
+      <c r="P6" s="1">
+        <f t="shared" si="1"/>
+        <v>7.163137025415435E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4773339521556203E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="1"/>
+        <v>4.619777425766549E-3</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9437107140334769E-3</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81717352920403985</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="1"/>
+        <v>6.7071726211495972E-2</v>
       </c>
       <c r="V6" s="1">
         <f>M6/$N6</f>
         <v>9.1572245820427194E-4</v>
       </c>
+      <c r="W6" s="51">
+        <f>SUM(L6,F6:H6)/N6</f>
+        <v>0.11189531141222644</v>
+      </c>
+      <c r="X6" s="1">
+        <f>SUM(I6:K6,M6)/N6</f>
+        <v>0.88810468858777358</v>
+      </c>
+      <c r="Y6" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
made changes to storm SSY tables
per Trent's feedback
</commit_message>
<xml_diff>
--- a/Data/LandCover/Watershed_Stats.xlsx
+++ b/Data/LandCover/Watershed_Stats.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t>Watershed</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>% Disturbed</t>
+  </si>
+  <si>
+    <t>LOWER (QUARRY+VILLAGE)</t>
   </si>
 </sst>
 </file>
@@ -668,7 +671,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
@@ -1347,13 +1350,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1623,7 @@
         <v>6.5460051025793137E-2</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X6" si="3">SUM(I3:K3)/N3</f>
+        <f t="shared" ref="X3:X5" si="3">SUM(I3:K3)/N3</f>
         <v>0.93453994897420689</v>
       </c>
       <c r="Y3" s="54"/>
@@ -1883,6 +1886,15 @@
         <v>0.88810468858777358</v>
       </c>
       <c r="Y6" s="54"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>47</v>
+      </c>
+      <c r="W8">
+        <f>(SUM(L3:L4)+SUM(G3:G4)+SUM(F3:F4))/SUM(N3:N4)</f>
+        <v>5.180927718982211E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed some of the Land Cover calculations
</commit_message>
<xml_diff>
--- a/Data/LandCover/Watershed_Stats.xlsx
+++ b/Data/LandCover/Watershed_Stats.xlsx
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Fagaalu" sheetId="1" r:id="rId1"/>
     <sheet name="Fagaalu_Revised" sheetId="3" r:id="rId2"/>
-    <sheet name="Nuuuli" sheetId="2" r:id="rId3"/>
+    <sheet name="Fagaalu_Revised_check" sheetId="4" r:id="rId3"/>
+    <sheet name="Nuuuli" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="54">
   <si>
     <t>Watershed</t>
   </si>
@@ -170,6 +171,24 @@
   </si>
   <si>
     <t>LOWER (QUARRY+VILLAGE)</t>
+  </si>
+  <si>
+    <t>LOWER_VILLAGE (FG3)</t>
+  </si>
+  <si>
+    <t>UPPER (FG1)</t>
+  </si>
+  <si>
+    <t>LOWER_QUARRY (FG2)</t>
+  </si>
+  <si>
+    <t>LOWER (FG3)</t>
+  </si>
+  <si>
+    <t>Subwatershed (pourpoint)</t>
+  </si>
+  <si>
+    <t>TOTAL (FG3)</t>
   </si>
 </sst>
 </file>
@@ -325,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -387,6 +406,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +691,10 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,10 +1373,730 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="48" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="31">
+        <v>0.89724999999999999</v>
+      </c>
+      <c r="C2" s="33">
+        <f>B2/$B$7</f>
+        <v>0.48221306911622125</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0.48</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="34">
+        <v>476</v>
+      </c>
+      <c r="J2" s="34">
+        <v>739484</v>
+      </c>
+      <c r="K2" s="34">
+        <v>153685</v>
+      </c>
+      <c r="L2" s="34">
+        <v>3574</v>
+      </c>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34">
+        <f t="shared" ref="N2:N8" si="0">SUM(F2:M2)</f>
+        <v>897219</v>
+      </c>
+      <c r="O2" s="35">
+        <f>L2/$N2</f>
+        <v>3.9834198785357868E-3</v>
+      </c>
+      <c r="P2" s="35">
+        <f t="shared" ref="P2:U8" si="1">F2/$N2</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R2" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S2" s="35">
+        <f t="shared" si="1"/>
+        <v>5.3052822109206333E-4</v>
+      </c>
+      <c r="T2" s="35">
+        <f t="shared" si="1"/>
+        <v>0.82419565345807433</v>
+      </c>
+      <c r="U2" s="35">
+        <f t="shared" si="1"/>
+        <v>0.17129039844229782</v>
+      </c>
+      <c r="V2" s="36">
+        <f>M2/$N2</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="51">
+        <f>SUM(L2,F2:G2)/N2</f>
+        <v>3.9834198785357868E-3</v>
+      </c>
+      <c r="X2" s="1">
+        <f>SUM(I2:K2)/N2</f>
+        <v>0.99601658012146421</v>
+      </c>
+      <c r="Y2" s="54"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1.171996</v>
+      </c>
+      <c r="C3" s="28">
+        <f>B3/$B$7</f>
+        <v>0.62987103722701021</v>
+      </c>
+      <c r="D3" s="26">
+        <v>0.27474600000000005</v>
+      </c>
+      <c r="E3" s="27">
+        <f>0.27/1.86</f>
+        <v>0.14516129032258066</v>
+      </c>
+      <c r="F3" s="25">
+        <f>2008-F2</f>
+        <v>2008</v>
+      </c>
+      <c r="G3" s="25">
+        <f>348-G2</f>
+        <v>348</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25">
+        <f>1816-I2</f>
+        <v>1340</v>
+      </c>
+      <c r="J3" s="25">
+        <f>992494-J2</f>
+        <v>253010</v>
+      </c>
+      <c r="K3" s="25">
+        <f>156112-K2</f>
+        <v>2427</v>
+      </c>
+      <c r="L3" s="25">
+        <f>19204-L2</f>
+        <v>15630</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25">
+        <f t="shared" si="0"/>
+        <v>274763</v>
+      </c>
+      <c r="O3" s="29">
+        <f>L3/$N3</f>
+        <v>5.6885388498451393E-2</v>
+      </c>
+      <c r="P3" s="29">
+        <f t="shared" si="1"/>
+        <v>7.3081164494491618E-3</v>
+      </c>
+      <c r="Q3" s="29">
+        <f t="shared" si="1"/>
+        <v>1.2665460778925838E-3</v>
+      </c>
+      <c r="R3" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S3" s="29">
+        <f t="shared" si="1"/>
+        <v>4.8769302999312134E-3</v>
+      </c>
+      <c r="T3" s="29">
+        <f t="shared" si="1"/>
+        <v>0.92082995163104198</v>
+      </c>
+      <c r="U3" s="29">
+        <f t="shared" si="1"/>
+        <v>8.8330670432336233E-3</v>
+      </c>
+      <c r="V3" s="30">
+        <f>M3/$N3</f>
+        <v>0</v>
+      </c>
+      <c r="W3" s="51">
+        <f t="shared" ref="W3:W4" si="2">SUM(L3,F3:G3)/N3</f>
+        <v>6.5460051025793137E-2</v>
+      </c>
+      <c r="X3" s="1">
+        <f t="shared" ref="X3:X7" si="3">SUM(I3:K3)/N3</f>
+        <v>0.93453994897420689</v>
+      </c>
+      <c r="Y3" s="54"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="37">
+        <v>1.776413</v>
+      </c>
+      <c r="C4" s="39">
+        <f>B4/$B$7</f>
+        <v>0.95470556115681693</v>
+      </c>
+      <c r="D4" s="37">
+        <f>B4-B3</f>
+        <v>0.60441699999999998</v>
+      </c>
+      <c r="E4" s="38">
+        <f>D4/1.86</f>
+        <v>0.324955376344086</v>
+      </c>
+      <c r="F4" s="40">
+        <f>56406-F2-F3</f>
+        <v>54398</v>
+      </c>
+      <c r="G4" s="40">
+        <f>16249-G2-G3</f>
+        <v>15901</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="40">
+        <f>2874-I2-I3</f>
+        <v>1058</v>
+      </c>
+      <c r="J4" s="40">
+        <f>1521947-J2-J3</f>
+        <v>529453</v>
+      </c>
+      <c r="K4" s="40">
+        <f>159545-K2-K3</f>
+        <v>3433</v>
+      </c>
+      <c r="L4" s="40">
+        <f>19379-L2-L3</f>
+        <v>175</v>
+      </c>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40">
+        <f>SUM(F4:M4)</f>
+        <v>604418</v>
+      </c>
+      <c r="O4" s="41">
+        <f>L4/$N4</f>
+        <v>2.8953472596779048E-4</v>
+      </c>
+      <c r="P4" s="41">
+        <f t="shared" si="1"/>
+        <v>9.000062870397639E-2</v>
+      </c>
+      <c r="Q4" s="41">
+        <f t="shared" si="1"/>
+        <v>2.6307952443507639E-2</v>
+      </c>
+      <c r="R4" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="41">
+        <f t="shared" si="1"/>
+        <v>1.750444228993842E-3</v>
+      </c>
+      <c r="T4" s="41">
+        <f t="shared" si="1"/>
+        <v>0.87597159581614048</v>
+      </c>
+      <c r="U4" s="41">
+        <f t="shared" si="1"/>
+        <v>5.6798440814138556E-3</v>
+      </c>
+      <c r="V4" s="42">
+        <f>M4/$N4</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="51">
+        <f t="shared" si="2"/>
+        <v>0.11659811587345181</v>
+      </c>
+      <c r="X4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.88340188412654819</v>
+      </c>
+      <c r="Y4" s="54"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="37">
+        <v>1.776413</v>
+      </c>
+      <c r="C5" s="39">
+        <f>B5/$B$7</f>
+        <v>0.95470556115681693</v>
+      </c>
+      <c r="D5" s="37">
+        <f>SUM(D3:D4)</f>
+        <v>0.87916300000000003</v>
+      </c>
+      <c r="E5" s="38">
+        <f>D5/1.86</f>
+        <v>0.47266827956989244</v>
+      </c>
+      <c r="F5" s="40">
+        <f>56406</f>
+        <v>56406</v>
+      </c>
+      <c r="G5" s="40">
+        <f>16249</f>
+        <v>16249</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="40">
+        <f>2874-I2</f>
+        <v>2398</v>
+      </c>
+      <c r="J5" s="40">
+        <f>1521947-J2</f>
+        <v>782463</v>
+      </c>
+      <c r="K5" s="40">
+        <f>159545-K2</f>
+        <v>5860</v>
+      </c>
+      <c r="L5" s="40">
+        <f>19379-L2</f>
+        <v>15805</v>
+      </c>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40">
+        <f>SUM(F5:M5)</f>
+        <v>879181</v>
+      </c>
+      <c r="O5" s="41">
+        <f>L5/$N5</f>
+        <v>1.7976958100777884E-2</v>
+      </c>
+      <c r="P5" s="41">
+        <f>F5/$N5</f>
+        <v>6.4157437433247533E-2</v>
+      </c>
+      <c r="Q5" s="41">
+        <f t="shared" ref="Q5" si="4">G5/$N5</f>
+        <v>1.8481973564032889E-2</v>
+      </c>
+      <c r="R5" s="41">
+        <f t="shared" ref="R5" si="5">H5/$N5</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="41">
+        <f t="shared" ref="S5" si="6">I5/$N5</f>
+        <v>2.7275384704628512E-3</v>
+      </c>
+      <c r="T5" s="41">
+        <f t="shared" ref="T5" si="7">J5/$N5</f>
+        <v>0.8899907982542844</v>
+      </c>
+      <c r="U5" s="41">
+        <f t="shared" ref="U5" si="8">K5/$N5</f>
+        <v>6.6652941771944575E-3</v>
+      </c>
+      <c r="V5" s="42">
+        <f>M5/$N5</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="51">
+        <f>SUM(L5,F5:G5)/N5</f>
+        <v>0.10061636909805831</v>
+      </c>
+      <c r="X5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89938363090194173</v>
+      </c>
+      <c r="Y5" s="54"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="37">
+        <v>1.776413</v>
+      </c>
+      <c r="C6" s="39">
+        <f>B6/$B$7</f>
+        <v>0.95470556115681693</v>
+      </c>
+      <c r="D6" s="37">
+        <v>1.78</v>
+      </c>
+      <c r="E6" s="38">
+        <f>D6/1.86</f>
+        <v>0.95698924731182788</v>
+      </c>
+      <c r="F6" s="40">
+        <f>SUM(F5,F2)</f>
+        <v>56406</v>
+      </c>
+      <c r="G6" s="40">
+        <f t="shared" ref="G6:N6" si="9">SUM(G5,G2)</f>
+        <v>16249</v>
+      </c>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40">
+        <f t="shared" si="9"/>
+        <v>2874</v>
+      </c>
+      <c r="J6" s="40">
+        <f t="shared" si="9"/>
+        <v>1521947</v>
+      </c>
+      <c r="K6" s="40">
+        <f t="shared" si="9"/>
+        <v>159545</v>
+      </c>
+      <c r="L6" s="40">
+        <f t="shared" si="9"/>
+        <v>19379</v>
+      </c>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40">
+        <f t="shared" si="9"/>
+        <v>1776400</v>
+      </c>
+      <c r="O6" s="41">
+        <f>L6/$N6</f>
+        <v>1.0909142085115965E-2</v>
+      </c>
+      <c r="P6" s="41">
+        <f>F6/$N6</f>
+        <v>3.175298356226075E-2</v>
+      </c>
+      <c r="Q6" s="41">
+        <f t="shared" ref="Q6" si="10">G6/$N6</f>
+        <v>9.1471515424453951E-3</v>
+      </c>
+      <c r="R6" s="41">
+        <f t="shared" ref="R6" si="11">H6/$N6</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="41">
+        <f t="shared" ref="S6" si="12">I6/$N6</f>
+        <v>1.6178788561134879E-3</v>
+      </c>
+      <c r="T6" s="41">
+        <f t="shared" ref="T6" si="13">J6/$N6</f>
+        <v>0.85675917586129247</v>
+      </c>
+      <c r="U6" s="41">
+        <f t="shared" ref="U6" si="14">K6/$N6</f>
+        <v>8.9813668092771901E-2</v>
+      </c>
+      <c r="V6" s="42">
+        <f>M6/$N6</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="51">
+        <f>SUM(L6,F6:G6)/N6</f>
+        <v>5.180927718982211E-2</v>
+      </c>
+      <c r="X6" s="1">
+        <f t="shared" ref="X6" si="15">SUM(I6:K6)/N6</f>
+        <v>0.94819072281017791</v>
+      </c>
+      <c r="Y6" s="54"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="43">
+        <v>1.860692</v>
+      </c>
+      <c r="C7" s="45">
+        <f>B7/$B$7</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="43">
+        <v>8.4278999999999993E-2</v>
+      </c>
+      <c r="E7" s="44">
+        <v>4.5294438843183099E-2</v>
+      </c>
+      <c r="F7" s="13">
+        <v>85528</v>
+      </c>
+      <c r="G7" s="13">
+        <v>21192</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>2874</v>
+      </c>
+      <c r="J7" s="13">
+        <v>1571530</v>
+      </c>
+      <c r="K7" s="13">
+        <v>160179</v>
+      </c>
+      <c r="L7" s="13">
+        <v>19379</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13">
+        <f>SUM(F7:M7)</f>
+        <v>1860682</v>
+      </c>
+      <c r="O7" s="46">
+        <f>L7/$N7</f>
+        <v>1.0414998371564834E-2</v>
+      </c>
+      <c r="P7" s="46">
+        <f t="shared" si="1"/>
+        <v>4.5965941520367266E-2</v>
+      </c>
+      <c r="Q7" s="46">
+        <f>G7/$N7</f>
+        <v>1.1389372283926001E-2</v>
+      </c>
+      <c r="R7" s="46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="46">
+        <f t="shared" si="1"/>
+        <v>1.5445949388450042E-3</v>
+      </c>
+      <c r="T7" s="46">
+        <f t="shared" si="1"/>
+        <v>0.84459891588138114</v>
+      </c>
+      <c r="U7" s="46">
+        <f t="shared" si="1"/>
+        <v>8.608617700391577E-2</v>
+      </c>
+      <c r="V7" s="47">
+        <f>M7/$N7</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="51">
+        <f>SUM(L7,F7:G7)/N7</f>
+        <v>6.7770312175858105E-2</v>
+      </c>
+      <c r="X7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.93222968782414195</v>
+      </c>
+      <c r="Y7" s="54"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2.4778150000000001</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="50"/>
+      <c r="F8">
+        <v>177490</v>
+      </c>
+      <c r="G8">
+        <v>61384</v>
+      </c>
+      <c r="H8">
+        <v>11447</v>
+      </c>
+      <c r="I8">
+        <v>7294</v>
+      </c>
+      <c r="J8">
+        <v>2024813</v>
+      </c>
+      <c r="K8">
+        <v>166192</v>
+      </c>
+      <c r="L8">
+        <v>26936</v>
+      </c>
+      <c r="M8">
+        <v>2269</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>2477825</v>
+      </c>
+      <c r="O8" s="1">
+        <f>L8/$N8</f>
+        <v>1.0870824210749346E-2</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="1"/>
+        <v>7.163137025415435E-2</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4773339521556203E-2</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.619777425766549E-3</v>
+      </c>
+      <c r="S8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9437107140334769E-3</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81717352920403985</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="1"/>
+        <v>6.7071726211495972E-2</v>
+      </c>
+      <c r="V8" s="1">
+        <f>M8/$N8</f>
+        <v>9.1572245820427194E-4</v>
+      </c>
+      <c r="W8" s="51">
+        <f>SUM(L8,F8:H8)/N8</f>
+        <v>0.11189531141222644</v>
+      </c>
+      <c r="X8" s="1">
+        <f>SUM(I8:K8,M8)/N8</f>
+        <v>0.88810468858777358</v>
+      </c>
+      <c r="Y8" s="54"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +2233,7 @@
       </c>
       <c r="M2" s="34"/>
       <c r="N2" s="34">
-        <f t="shared" ref="N2:N6" si="0">SUM(F2:M2)</f>
+        <f>SUM(F2:M2)</f>
         <v>897219</v>
       </c>
       <c r="O2" s="35">
@@ -1501,27 +2241,27 @@
         <v>3.9834198785357868E-3</v>
       </c>
       <c r="P2" s="35">
-        <f t="shared" ref="P2:U6" si="1">F2/$N2</f>
+        <f t="shared" ref="P2:U6" si="0">F2/$N2</f>
         <v>0</v>
       </c>
       <c r="Q2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.3052822109206333E-4</v>
       </c>
       <c r="T2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.82419565345807433</v>
       </c>
       <c r="U2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.17129039844229782</v>
       </c>
       <c r="V2" s="36">
@@ -1583,7 +2323,7 @@
       </c>
       <c r="M3" s="25"/>
       <c r="N3" s="25">
-        <f t="shared" si="0"/>
+        <f>SUM(F3:M3)</f>
         <v>274763</v>
       </c>
       <c r="O3" s="29">
@@ -1591,27 +2331,27 @@
         <v>5.6885388498451393E-2</v>
       </c>
       <c r="P3" s="29">
-        <f t="shared" si="1"/>
+        <f>F3/$N3</f>
         <v>7.3081164494491618E-3</v>
       </c>
       <c r="Q3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2665460778925838E-3</v>
       </c>
       <c r="R3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.8769302999312134E-3</v>
       </c>
       <c r="T3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.92082995163104198</v>
       </c>
       <c r="U3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.8330670432336233E-3</v>
       </c>
       <c r="V3" s="30">
@@ -1619,11 +2359,11 @@
         <v>0</v>
       </c>
       <c r="W3" s="51">
-        <f t="shared" ref="W3:W5" si="2">SUM(L3,F3:G3)/N3</f>
+        <f>SUM(L3,F3:G3)/N3</f>
         <v>6.5460051025793137E-2</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X5" si="3">SUM(I3:K3)/N3</f>
+        <f t="shared" ref="X3:X5" si="1">SUM(I3:K3)/N3</f>
         <v>0.93453994897420689</v>
       </c>
       <c r="Y3" s="54"/>
@@ -1657,65 +2397,65 @@
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="40">
-        <f>2874-I3</f>
-        <v>1534</v>
+        <f>2874-I3-I2</f>
+        <v>1058</v>
       </c>
       <c r="J4" s="40">
-        <f>1521947-J3</f>
-        <v>1268937</v>
+        <f>1521947-J2-J3</f>
+        <v>529453</v>
       </c>
       <c r="K4" s="40">
-        <f>159545-K3</f>
-        <v>157118</v>
+        <f>159545-K3-K2</f>
+        <v>3433</v>
       </c>
       <c r="L4" s="40">
-        <f>19379-L3</f>
-        <v>3749</v>
+        <f>19379-L3-L2</f>
+        <v>175</v>
       </c>
       <c r="M4" s="40"/>
       <c r="N4" s="40">
-        <f t="shared" si="0"/>
-        <v>1501637</v>
+        <f>SUM(F4:M4)</f>
+        <v>604418</v>
       </c>
       <c r="O4" s="41">
         <f>L4/$N4</f>
-        <v>2.4966087010376008E-3</v>
+        <v>2.8953472596779048E-4</v>
       </c>
       <c r="P4" s="41">
-        <f t="shared" si="1"/>
-        <v>3.6225798911454631E-2</v>
+        <f>F4/$N4</f>
+        <v>9.000062870397639E-2</v>
       </c>
       <c r="Q4" s="41">
-        <f t="shared" si="1"/>
-        <v>1.0589110417497704E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.6307952443507639E-2</v>
       </c>
       <c r="R4" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S4" s="41">
-        <f t="shared" si="1"/>
-        <v>1.0215518131212803E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.750444228993842E-3</v>
       </c>
       <c r="T4" s="41">
-        <f t="shared" si="1"/>
-        <v>0.84503578428075499</v>
+        <f t="shared" si="0"/>
+        <v>0.87597159581614048</v>
       </c>
       <c r="U4" s="41">
-        <f t="shared" si="1"/>
-        <v>0.10463114587613384</v>
+        <f t="shared" si="0"/>
+        <v>5.6798440814138556E-3</v>
       </c>
       <c r="V4" s="42">
         <f>M4/$N4</f>
         <v>0</v>
       </c>
       <c r="W4" s="51">
-        <f t="shared" si="2"/>
-        <v>4.931151802998994E-2</v>
+        <f t="shared" ref="W4:W5" si="2">SUM(L4,F4:G4)/N4</f>
+        <v>0.11659811587345181</v>
       </c>
       <c r="X4" s="1">
-        <f t="shared" si="3"/>
-        <v>0.9506884819700101</v>
+        <f t="shared" si="1"/>
+        <v>0.88340188412654819</v>
       </c>
       <c r="Y4" s="54"/>
     </row>
@@ -1757,7 +2497,7 @@
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13">
-        <f t="shared" si="0"/>
+        <f>SUM(F5:M5)</f>
         <v>1860682</v>
       </c>
       <c r="O5" s="46">
@@ -1765,27 +2505,27 @@
         <v>1.0414998371564834E-2</v>
       </c>
       <c r="P5" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.5965941520367266E-2</v>
       </c>
       <c r="Q5" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1389372283926001E-2</v>
       </c>
       <c r="R5" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S5" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5445949388450042E-3</v>
       </c>
       <c r="T5" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.84459891588138114</v>
       </c>
       <c r="U5" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.608617700391577E-2</v>
       </c>
       <c r="V5" s="47">
@@ -1797,7 +2537,7 @@
         <v>6.7770312175858105E-2</v>
       </c>
       <c r="X5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0.93222968782414195</v>
       </c>
       <c r="Y5" s="54"/>
@@ -1842,7 +2582,7 @@
         <v>2269</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f>SUM(F6:M6)</f>
         <v>2477825</v>
       </c>
       <c r="O6" s="1">
@@ -1850,27 +2590,27 @@
         <v>1.0870824210749346E-2</v>
       </c>
       <c r="P6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7.163137025415435E-2</v>
       </c>
       <c r="Q6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.4773339521556203E-2</v>
       </c>
       <c r="R6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.619777425766549E-3</v>
       </c>
       <c r="S6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.9437107140334769E-3</v>
       </c>
       <c r="T6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.81717352920403985</v>
       </c>
       <c r="U6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.7071726211495972E-2</v>
       </c>
       <c r="V6" s="1">
@@ -1888,12 +2628,14 @@
       <c r="Y6" s="54"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="55"/>
+      <c r="D8" s="3"/>
       <c r="V8" t="s">
         <v>47</v>
       </c>
       <c r="W8">
         <f>(SUM(L3:L4)+SUM(G3:G4)+SUM(F3:F4))/SUM(N3:N4)</f>
-        <v>5.180927718982211E-2</v>
+        <v>0.10061636909805831</v>
       </c>
     </row>
   </sheetData>
@@ -1902,7 +2644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>

</xml_diff>

<commit_message>
got the htmlTables working much better
I can finally borrow code from Trent , just for R
</commit_message>
<xml_diff>
--- a/Data/LandCover/Watershed_Stats.xlsx
+++ b/Data/LandCover/Watershed_Stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
   <si>
     <t>Watershed</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>TOTAL (FG3)</t>
+  </si>
+  <si>
+    <t>Fagaalu Watershed (outlet to ocean)</t>
   </si>
 </sst>
 </file>
@@ -1373,10 +1376,10 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1497,8 @@
         <v>0.9</v>
       </c>
       <c r="E2" s="32">
-        <v>0.48</v>
+        <f>C2</f>
+        <v>0.48221306911622125</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
@@ -1517,35 +1521,35 @@
         <v>897219</v>
       </c>
       <c r="O2" s="35">
-        <f>L2/$N2</f>
+        <f t="shared" ref="O2:O8" si="1">L2/$N2</f>
         <v>3.9834198785357868E-3</v>
       </c>
       <c r="P2" s="35">
-        <f t="shared" ref="P2:U8" si="1">F2/$N2</f>
+        <f t="shared" ref="P2:U8" si="2">F2/$N2</f>
         <v>0</v>
       </c>
       <c r="Q2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.3052822109206333E-4</v>
       </c>
       <c r="T2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.82419565345807433</v>
       </c>
       <c r="U2" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17129039844229782</v>
       </c>
       <c r="V2" s="36">
-        <f>M2/$N2</f>
+        <f t="shared" ref="V2:V8" si="3">M2/$N2</f>
         <v>0</v>
       </c>
       <c r="W2" s="51">
@@ -1566,7 +1570,7 @@
         <v>1.171996</v>
       </c>
       <c r="C3" s="28">
-        <f>B3/$B$7</f>
+        <f t="shared" ref="C2:C7" si="4">B3/$B$7</f>
         <v>0.62987103722701021</v>
       </c>
       <c r="D3" s="26">
@@ -1607,43 +1611,43 @@
         <v>274763</v>
       </c>
       <c r="O3" s="29">
-        <f>L3/$N3</f>
+        <f t="shared" si="1"/>
         <v>5.6885388498451393E-2</v>
       </c>
       <c r="P3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3081164494491618E-3</v>
       </c>
       <c r="Q3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2665460778925838E-3</v>
       </c>
       <c r="R3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.8769302999312134E-3</v>
       </c>
       <c r="T3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92082995163104198</v>
       </c>
       <c r="U3" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8330670432336233E-3</v>
       </c>
       <c r="V3" s="30">
-        <f>M3/$N3</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W3" s="51">
-        <f t="shared" ref="W3:W4" si="2">SUM(L3,F3:G3)/N3</f>
+        <f t="shared" ref="W3:W4" si="5">SUM(L3,F3:G3)/N3</f>
         <v>6.5460051025793137E-2</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X7" si="3">SUM(I3:K3)/N3</f>
+        <f t="shared" ref="X3:X7" si="6">SUM(I3:K3)/N3</f>
         <v>0.93453994897420689</v>
       </c>
       <c r="Y3" s="54"/>
@@ -1656,7 +1660,7 @@
         <v>1.776413</v>
       </c>
       <c r="C4" s="39">
-        <f>B4/$B$7</f>
+        <f t="shared" si="4"/>
         <v>0.95470556115681693</v>
       </c>
       <c r="D4" s="37">
@@ -1698,43 +1702,43 @@
         <v>604418</v>
       </c>
       <c r="O4" s="41">
-        <f>L4/$N4</f>
+        <f t="shared" si="1"/>
         <v>2.8953472596779048E-4</v>
       </c>
       <c r="P4" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.000062870397639E-2</v>
       </c>
       <c r="Q4" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6307952443507639E-2</v>
       </c>
       <c r="R4" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S4" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.750444228993842E-3</v>
       </c>
       <c r="T4" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.87597159581614048</v>
       </c>
       <c r="U4" s="41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.6798440814138556E-3</v>
       </c>
       <c r="V4" s="42">
-        <f>M4/$N4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W4" s="51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.11659811587345181</v>
       </c>
       <c r="X4" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.88340188412654819</v>
       </c>
       <c r="Y4" s="54"/>
@@ -1747,7 +1751,7 @@
         <v>1.776413</v>
       </c>
       <c r="C5" s="39">
-        <f>B5/$B$7</f>
+        <f t="shared" si="4"/>
         <v>0.95470556115681693</v>
       </c>
       <c r="D5" s="37">
@@ -1789,7 +1793,7 @@
         <v>879181</v>
       </c>
       <c r="O5" s="41">
-        <f>L5/$N5</f>
+        <f t="shared" si="1"/>
         <v>1.7976958100777884E-2</v>
       </c>
       <c r="P5" s="41">
@@ -1797,27 +1801,27 @@
         <v>6.4157437433247533E-2</v>
       </c>
       <c r="Q5" s="41">
-        <f t="shared" ref="Q5" si="4">G5/$N5</f>
+        <f t="shared" ref="Q5" si="7">G5/$N5</f>
         <v>1.8481973564032889E-2</v>
       </c>
       <c r="R5" s="41">
-        <f t="shared" ref="R5" si="5">H5/$N5</f>
+        <f t="shared" ref="R5" si="8">H5/$N5</f>
         <v>0</v>
       </c>
       <c r="S5" s="41">
-        <f t="shared" ref="S5" si="6">I5/$N5</f>
+        <f t="shared" ref="S5" si="9">I5/$N5</f>
         <v>2.7275384704628512E-3</v>
       </c>
       <c r="T5" s="41">
-        <f t="shared" ref="T5" si="7">J5/$N5</f>
+        <f t="shared" ref="T5" si="10">J5/$N5</f>
         <v>0.8899907982542844</v>
       </c>
       <c r="U5" s="41">
-        <f t="shared" ref="U5" si="8">K5/$N5</f>
+        <f t="shared" ref="U5" si="11">K5/$N5</f>
         <v>6.6652941771944575E-3</v>
       </c>
       <c r="V5" s="42">
-        <f>M5/$N5</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W5" s="51">
@@ -1825,7 +1829,7 @@
         <v>0.10061636909805831</v>
       </c>
       <c r="X5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.89938363090194173</v>
       </c>
       <c r="Y5" s="54"/>
@@ -1838,7 +1842,7 @@
         <v>1.776413</v>
       </c>
       <c r="C6" s="39">
-        <f>B6/$B$7</f>
+        <f t="shared" si="4"/>
         <v>0.95470556115681693</v>
       </c>
       <c r="D6" s="37">
@@ -1853,33 +1857,33 @@
         <v>56406</v>
       </c>
       <c r="G6" s="40">
-        <f t="shared" ref="G6:N6" si="9">SUM(G5,G2)</f>
+        <f t="shared" ref="G6:N6" si="12">SUM(G5,G2)</f>
         <v>16249</v>
       </c>
       <c r="H6" s="40"/>
       <c r="I6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2874</v>
       </c>
       <c r="J6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1521947</v>
       </c>
       <c r="K6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>159545</v>
       </c>
       <c r="L6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>19379</v>
       </c>
       <c r="M6" s="40"/>
       <c r="N6" s="40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>1776400</v>
       </c>
       <c r="O6" s="41">
-        <f>L6/$N6</f>
+        <f t="shared" si="1"/>
         <v>1.0909142085115965E-2</v>
       </c>
       <c r="P6" s="41">
@@ -1887,27 +1891,27 @@
         <v>3.175298356226075E-2</v>
       </c>
       <c r="Q6" s="41">
-        <f t="shared" ref="Q6" si="10">G6/$N6</f>
+        <f t="shared" ref="Q6" si="13">G6/$N6</f>
         <v>9.1471515424453951E-3</v>
       </c>
       <c r="R6" s="41">
-        <f t="shared" ref="R6" si="11">H6/$N6</f>
+        <f t="shared" ref="R6" si="14">H6/$N6</f>
         <v>0</v>
       </c>
       <c r="S6" s="41">
-        <f t="shared" ref="S6" si="12">I6/$N6</f>
+        <f t="shared" ref="S6" si="15">I6/$N6</f>
         <v>1.6178788561134879E-3</v>
       </c>
       <c r="T6" s="41">
-        <f t="shared" ref="T6" si="13">J6/$N6</f>
+        <f t="shared" ref="T6" si="16">J6/$N6</f>
         <v>0.85675917586129247</v>
       </c>
       <c r="U6" s="41">
-        <f t="shared" ref="U6" si="14">K6/$N6</f>
+        <f t="shared" ref="U6" si="17">K6/$N6</f>
         <v>8.9813668092771901E-2</v>
       </c>
       <c r="V6" s="42">
-        <f>M6/$N6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W6" s="51">
@@ -1915,20 +1919,20 @@
         <v>5.180927718982211E-2</v>
       </c>
       <c r="X6" s="1">
-        <f t="shared" ref="X6" si="15">SUM(I6:K6)/N6</f>
+        <f t="shared" ref="X6" si="18">SUM(I6:K6)/N6</f>
         <v>0.94819072281017791</v>
       </c>
       <c r="Y6" s="54"/>
     </row>
     <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B7" s="43">
         <v>1.860692</v>
       </c>
       <c r="C7" s="45">
-        <f>B7/$B$7</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="D7" s="43">
@@ -1962,11 +1966,11 @@
         <v>1860682</v>
       </c>
       <c r="O7" s="46">
-        <f>L7/$N7</f>
+        <f t="shared" si="1"/>
         <v>1.0414998371564834E-2</v>
       </c>
       <c r="P7" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5965941520367266E-2</v>
       </c>
       <c r="Q7" s="46">
@@ -1974,23 +1978,23 @@
         <v>1.1389372283926001E-2</v>
       </c>
       <c r="R7" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S7" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5445949388450042E-3</v>
       </c>
       <c r="T7" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.84459891588138114</v>
       </c>
       <c r="U7" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.608617700391577E-2</v>
       </c>
       <c r="V7" s="47">
-        <f>M7/$N7</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W7" s="51">
@@ -1998,7 +2002,7 @@
         <v>6.7770312175858105E-2</v>
       </c>
       <c r="X7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.93222968782414195</v>
       </c>
       <c r="Y7" s="54"/>
@@ -2041,35 +2045,35 @@
         <v>2477825</v>
       </c>
       <c r="O8" s="1">
-        <f>L8/$N8</f>
+        <f t="shared" si="1"/>
         <v>1.0870824210749346E-2</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.163137025415435E-2</v>
       </c>
       <c r="Q8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4773339521556203E-2</v>
       </c>
       <c r="R8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.619777425766549E-3</v>
       </c>
       <c r="S8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9437107140334769E-3</v>
       </c>
       <c r="T8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81717352920403985</v>
       </c>
       <c r="U8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7071726211495972E-2</v>
       </c>
       <c r="V8" s="1">
-        <f>M8/$N8</f>
+        <f t="shared" si="3"/>
         <v>9.1572245820427194E-4</v>
       </c>
       <c r="W8" s="51">

</xml_diff>

<commit_message>
Revised storm definition in manuscript
going to hack apart the data collection methods and results
</commit_message>
<xml_diff>
--- a/Data/LandCover/Watershed_Stats.xlsx
+++ b/Data/LandCover/Watershed_Stats.xlsx
@@ -1376,10 +1376,10 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,15 +1490,15 @@
         <v>0.89724999999999999</v>
       </c>
       <c r="C2" s="33">
-        <f>B2/$B$7</f>
-        <v>0.48221306911622125</v>
+        <f>B2/$B$6</f>
+        <v>0.50509087695260058</v>
       </c>
       <c r="D2" s="31">
         <v>0.9</v>
       </c>
       <c r="E2" s="32">
         <f>C2</f>
-        <v>0.48221306911622125</v>
+        <v>0.50509087695260058</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
@@ -1569,16 +1569,16 @@
       <c r="B3" s="26">
         <v>1.171996</v>
       </c>
-      <c r="C3" s="28">
-        <f t="shared" ref="C2:C7" si="4">B3/$B$7</f>
-        <v>0.62987103722701021</v>
+      <c r="C3" s="33">
+        <f t="shared" ref="C3:C6" si="4">B3/$B$6</f>
+        <v>0.6597542350793425</v>
       </c>
       <c r="D3" s="26">
         <v>0.27474600000000005</v>
       </c>
       <c r="E3" s="27">
-        <f>0.27/1.86</f>
-        <v>0.14516129032258066</v>
+        <f>D3/$B$6</f>
+        <v>0.15466335812674195</v>
       </c>
       <c r="F3" s="25">
         <f>2008-F2</f>
@@ -1659,17 +1659,17 @@
       <c r="B4" s="37">
         <v>1.776413</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="33">
         <f t="shared" si="4"/>
-        <v>0.95470556115681693</v>
+        <v>1</v>
       </c>
       <c r="D4" s="37">
         <f>B4-B3</f>
         <v>0.60441699999999998</v>
       </c>
       <c r="E4" s="38">
-        <f>D4/1.86</f>
-        <v>0.324955376344086</v>
+        <f t="shared" ref="E4:E6" si="7">D4/$B$6</f>
+        <v>0.3402457649206575</v>
       </c>
       <c r="F4" s="40">
         <f>56406-F2-F3</f>
@@ -1750,17 +1750,17 @@
       <c r="B5" s="37">
         <v>1.776413</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="33">
         <f t="shared" si="4"/>
-        <v>0.95470556115681693</v>
+        <v>1</v>
       </c>
       <c r="D5" s="37">
         <f>SUM(D3:D4)</f>
         <v>0.87916300000000003</v>
       </c>
       <c r="E5" s="38">
-        <f>D5/1.86</f>
-        <v>0.47266827956989244</v>
+        <f t="shared" si="7"/>
+        <v>0.49490912304739948</v>
       </c>
       <c r="F5" s="40">
         <f>56406</f>
@@ -1801,23 +1801,23 @@
         <v>6.4157437433247533E-2</v>
       </c>
       <c r="Q5" s="41">
-        <f t="shared" ref="Q5" si="7">G5/$N5</f>
+        <f t="shared" ref="Q5" si="8">G5/$N5</f>
         <v>1.8481973564032889E-2</v>
       </c>
       <c r="R5" s="41">
-        <f t="shared" ref="R5" si="8">H5/$N5</f>
+        <f t="shared" ref="R5" si="9">H5/$N5</f>
         <v>0</v>
       </c>
       <c r="S5" s="41">
-        <f t="shared" ref="S5" si="9">I5/$N5</f>
+        <f t="shared" ref="S5" si="10">I5/$N5</f>
         <v>2.7275384704628512E-3</v>
       </c>
       <c r="T5" s="41">
-        <f t="shared" ref="T5" si="10">J5/$N5</f>
+        <f t="shared" ref="T5" si="11">J5/$N5</f>
         <v>0.8899907982542844</v>
       </c>
       <c r="U5" s="41">
-        <f t="shared" ref="U5" si="11">K5/$N5</f>
+        <f t="shared" ref="U5" si="12">K5/$N5</f>
         <v>6.6652941771944575E-3</v>
       </c>
       <c r="V5" s="42">
@@ -1841,49 +1841,49 @@
       <c r="B6" s="37">
         <v>1.776413</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="33">
         <f t="shared" si="4"/>
-        <v>0.95470556115681693</v>
+        <v>1</v>
       </c>
       <c r="D6" s="37">
         <v>1.78</v>
       </c>
       <c r="E6" s="38">
-        <f>D6/1.86</f>
-        <v>0.95698924731182788</v>
+        <f t="shared" si="7"/>
+        <v>1.0020192376434984</v>
       </c>
       <c r="F6" s="40">
         <f>SUM(F5,F2)</f>
         <v>56406</v>
       </c>
       <c r="G6" s="40">
-        <f t="shared" ref="G6:N6" si="12">SUM(G5,G2)</f>
+        <f t="shared" ref="G6:N6" si="13">SUM(G5,G2)</f>
         <v>16249</v>
       </c>
       <c r="H6" s="40"/>
       <c r="I6" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2874</v>
       </c>
       <c r="J6" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1521947</v>
       </c>
       <c r="K6" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>159545</v>
       </c>
       <c r="L6" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>19379</v>
       </c>
       <c r="M6" s="40"/>
       <c r="N6" s="40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1776400</v>
       </c>
       <c r="O6" s="41">
-        <f t="shared" si="1"/>
+        <f>L6/$N6</f>
         <v>1.0909142085115965E-2</v>
       </c>
       <c r="P6" s="41">
@@ -1891,23 +1891,23 @@
         <v>3.175298356226075E-2</v>
       </c>
       <c r="Q6" s="41">
-        <f t="shared" ref="Q6" si="13">G6/$N6</f>
+        <f t="shared" ref="Q6" si="14">G6/$N6</f>
         <v>9.1471515424453951E-3</v>
       </c>
       <c r="R6" s="41">
-        <f t="shared" ref="R6" si="14">H6/$N6</f>
+        <f t="shared" ref="R6" si="15">H6/$N6</f>
         <v>0</v>
       </c>
       <c r="S6" s="41">
-        <f t="shared" ref="S6" si="15">I6/$N6</f>
+        <f t="shared" ref="S6" si="16">I6/$N6</f>
         <v>1.6178788561134879E-3</v>
       </c>
       <c r="T6" s="41">
-        <f t="shared" ref="T6" si="16">J6/$N6</f>
+        <f t="shared" ref="T6" si="17">J6/$N6</f>
         <v>0.85675917586129247</v>
       </c>
       <c r="U6" s="41">
-        <f t="shared" ref="U6" si="17">K6/$N6</f>
+        <f t="shared" ref="U6" si="18">K6/$N6</f>
         <v>8.9813668092771901E-2</v>
       </c>
       <c r="V6" s="42">
@@ -1919,7 +1919,7 @@
         <v>5.180927718982211E-2</v>
       </c>
       <c r="X6" s="1">
-        <f t="shared" ref="X6" si="18">SUM(I6:K6)/N6</f>
+        <f t="shared" ref="X6" si="19">SUM(I6:K6)/N6</f>
         <v>0.94819072281017791</v>
       </c>
       <c r="Y6" s="54"/>
@@ -1932,7 +1932,7 @@
         <v>1.860692</v>
       </c>
       <c r="C7" s="45">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="C3:C7" si="20">B7/$B$7</f>
         <v>1</v>
       </c>
       <c r="D7" s="43">

</xml_diff>